<commit_message>
add until User Interface
</commit_message>
<xml_diff>
--- a/docs/Requirements.xlsx
+++ b/docs/Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dell-my.sharepoint.com/personal/roi_tiefenbrunn_dell_com/Documents/Desktop/Exam-Management-System/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ofek\Desktop\Univarsity\Exam-Management-System\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="11_F25DC773A252ABDACC104828F15F59725BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEF0D1AF-EC9D-4F67-9B54-EB271FC32678}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF3943B-A60C-4CCD-A50F-A17C3332EADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Requirement</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Watch pending tasks</t>
   </si>
   <si>
-    <t>Create tasks (if role permits)</t>
-  </si>
-  <si>
     <t>Ask for work</t>
   </si>
   <si>
@@ -63,13 +60,85 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Workflow Management:</t>
-  </si>
-  <si>
     <t>Exam Management:</t>
   </si>
   <si>
     <t>User Management:</t>
+  </si>
+  <si>
+    <t>SystemAdministor</t>
+  </si>
+  <si>
+    <t>Manage WMS at the dept/university level</t>
+  </si>
+  <si>
+    <t>Migrate, install, update, manage WMS system</t>
+  </si>
+  <si>
+    <t>Manage courses in WMS</t>
+  </si>
+  <si>
+    <t>Create new course entry in WMS</t>
+  </si>
+  <si>
+    <t>Backup and remove course entry in WMS</t>
+  </si>
+  <si>
+    <t>Remove, change roles per course (when course staff changes)</t>
+  </si>
+  <si>
+    <t>Assign roles to courses</t>
+  </si>
+  <si>
+    <t>Define course staff</t>
+  </si>
+  <si>
+    <t>Create tasks</t>
+  </si>
+  <si>
+    <t>Course Administrator</t>
+  </si>
+  <si>
+    <t>Assign roles to course staff</t>
+  </si>
+  <si>
+    <t>Define exam</t>
+  </si>
+  <si>
+    <t>Generate exam documents</t>
+  </si>
+  <si>
+    <t>Inspect changes by course staff</t>
+  </si>
+  <si>
+    <t>Course Staff</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Roles (Junior, Associate, Senior)</t>
+  </si>
+  <si>
+    <t>People (Instructores TAs  Graders)</t>
+  </si>
+  <si>
+    <t>Workflow Management Activities:</t>
+  </si>
+  <si>
+    <t>Log into system</t>
+  </si>
+  <si>
+    <t>All Users</t>
+  </si>
+  <si>
+    <t>Perform specific task</t>
+  </si>
+  <si>
+    <t>Ask for a task</t>
+  </si>
+  <si>
+    <t>What controls urgency</t>
   </si>
 </sst>
 </file>
@@ -111,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -122,11 +191,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,16 +475,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="4" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="50.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -430,79 +498,206 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>